<commit_message>
Corrección del error cantidadDeCompras de user en null y agregué link al botón de carga desde excel
</commit_message>
<xml_diff>
--- a/ecommercesportsDEV/src/main/resources/ArchivoExcel/productos.xlsx
+++ b/ecommercesportsDEV/src/main/resources/ArchivoExcel/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Licenciatura en Sistemas\3º AÑO\2º Cuatrimestre\Proyecto de Software\TP cuatrimesatral\MASTER\DESCARGAR - SUBIR A GIT\Ecommerce-Sports\ecommercesportsDEV\src\main\resources\ArchivoExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394BBDF6-16BA-436C-BF77-8773DF2D91E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65003B86-AC90-4B63-A235-990E6DEAB48F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Salomon</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>/img/products/salomon.jpg</t>
+  </si>
+  <si>
+    <t>Peso</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,12 +505,13 @@
     <col min="9" max="9" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="1"/>
-    <col min="13" max="13" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="1"/>
+    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -542,13 +546,16 @@
         <v>20</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -583,13 +590,16 @@
         <v>0</v>
       </c>
       <c r="L2" s="1">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -624,13 +634,16 @@
         <v>0</v>
       </c>
       <c r="L3" s="1">
+        <v>4</v>
+      </c>
+      <c r="M3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -665,13 +678,16 @@
         <v>0</v>
       </c>
       <c r="L4" s="1">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -708,11 +724,14 @@
       <c r="L5" s="1">
         <v>1</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -747,13 +766,16 @@
         <v>0</v>
       </c>
       <c r="L6" s="1">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,14 +810,17 @@
         <v>0</v>
       </c>
       <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1">
         <v>1</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LoRoMmpKthHLZIXgYMlenjpwIkyYUqhymr0M9S3ZKLYHr4J8O305g/w9HusTX3/9YEWD6QIol4mMjfMzt45MjQ==" saltValue="giYZKiGVQWRJ5s4/JlU4HQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oyvAfkTygoncmD4QsFc8yIGveWA3Y5Y1WFGJPJWyrd7NcyqwzFwUUf6hq8NyBkrCoeLLijULsD3FNTB9IQuRRQ==" saltValue="nMllqwUsoCB7QdGrA92i1A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>